<commit_message>
Implemented TestNG and parameterised testing.
Next stage is to implement the asserts.
</commit_message>
<xml_diff>
--- a/src/test/java/utilities/ExcelData.xlsx
+++ b/src/test/java/utilities/ExcelData.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26722"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="26200" windowHeight="13800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22905" windowHeight="12975"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginTests" sheetId="1" r:id="rId1"/>
+    <sheet name="flightsSearch" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,24 +22,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
-  <si>
-    <t>Invalid_Login</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>test@email.com</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>email@email.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+  <si>
+    <t>searchFlightsDataExcel</t>
+  </si>
+  <si>
+    <t>originCity</t>
+  </si>
+  <si>
+    <t>destinationCity</t>
+  </si>
+  <si>
+    <t>departureDate</t>
+  </si>
+  <si>
+    <t>returnDate</t>
+  </si>
+  <si>
+    <t>numOfAdults</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Mexico City</t>
+  </si>
+  <si>
+    <t>01/05/2016</t>
+  </si>
+  <si>
+    <t>06/05/2016</t>
+  </si>
+  <si>
+    <t>01/06/2016</t>
+  </si>
+  <si>
+    <t>07/06/2016</t>
+  </si>
+  <si>
+    <t>01/07/2016</t>
+  </si>
+  <si>
+    <t>08/07/2016</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -48,7 +94,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +125,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -95,7 +147,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -123,14 +175,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -151,6 +208,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -199,7 +259,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,7 +294,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -446,66 +506,114 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="B2" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="B3" s="6" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="6:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="6:7">
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F19" s="2"/>
       <c r="G19" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -522,7 +630,7 @@
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -539,7 +647,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
1April - Friday, heading home.
</commit_message>
<xml_diff>
--- a/src/test/java/utilities/ExcelData.xlsx
+++ b/src/test/java/utilities/ExcelData.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>searchFlightsDataExcel</t>
   </si>
@@ -506,7 +505,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,8 +543,8 @@
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>12</v>
@@ -602,6 +601,11 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="18" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F18" s="2"/>

</xml_diff>